<commit_message>
correct 2025 CWC missing team names
via claude: https://claude.ai/share/af0d4a76-94f8-470a-912f-a0e8dba8a765
</commit_message>
<xml_diff>
--- a/src/stp/database/2025-mens-club-world-cup.xlsx
+++ b/src/stp/database/2025-mens-club-world-cup.xlsx
@@ -3298,6 +3298,16 @@
         <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v/>
       </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>PAL</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>BOT</t>
+        </is>
+      </c>
       <c r="J50" s="2" t="n">
         <v>1</v>
       </c>
@@ -3338,6 +3348,16 @@
         <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v/>
       </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>SLB</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>CHE</t>
+        </is>
+      </c>
       <c r="J51" s="2" t="n">
         <v>1</v>
       </c>
@@ -3378,6 +3398,16 @@
         <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v/>
       </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>PSG</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>MIA</t>
+        </is>
+      </c>
       <c r="J52" s="2" t="n">
         <v>4</v>
       </c>
@@ -3416,6 +3446,16 @@
         <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v/>
       </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>FLA</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>BAY</t>
+        </is>
+      </c>
       <c r="J53" s="2" t="n">
         <v>2</v>
       </c>
@@ -3454,6 +3494,16 @@
         <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v/>
       </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>INT</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>FLU</t>
+        </is>
+      </c>
       <c r="J54" s="2" t="n">
         <v>0</v>
       </c>
@@ -3492,6 +3542,16 @@
         <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v/>
       </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>MCI</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>HIL</t>
+        </is>
+      </c>
       <c r="J55" s="2" t="n">
         <v>3</v>
       </c>
@@ -3532,6 +3592,16 @@
         <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v/>
       </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>RMA</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>JUV</t>
+        </is>
+      </c>
       <c r="J56" s="2" t="n">
         <v>1</v>
       </c>
@@ -3570,6 +3640,16 @@
         <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v/>
       </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>BVB</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>CFM</t>
+        </is>
+      </c>
       <c r="J57" s="2" t="n">
         <v>2</v>
       </c>
@@ -3608,6 +3688,16 @@
         <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v/>
       </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>FLU</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>HIL</t>
+        </is>
+      </c>
       <c r="J58" s="2" t="n">
         <v>2</v>
       </c>
@@ -3646,6 +3736,16 @@
         <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v/>
       </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>PAL</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>CHE</t>
+        </is>
+      </c>
       <c r="J59" s="2" t="n">
         <v>1</v>
       </c>
@@ -3684,6 +3784,16 @@
         <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v/>
       </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>PSG</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>BAY</t>
+        </is>
+      </c>
       <c r="J60" s="2" t="n">
         <v>2</v>
       </c>
@@ -3722,6 +3832,16 @@
         <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v/>
       </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>RMA</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>BVB</t>
+        </is>
+      </c>
       <c r="J61" s="2" t="n">
         <v>3</v>
       </c>
@@ -3760,6 +3880,16 @@
         <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v/>
       </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>FLU</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>CHE</t>
+        </is>
+      </c>
       <c r="J62" s="2" t="n">
         <v>0</v>
       </c>
@@ -3798,6 +3928,16 @@
         <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v/>
       </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>PSG</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>RMA</t>
+        </is>
+      </c>
       <c r="J63" s="2" t="n">
         <v>4</v>
       </c>
@@ -3835,6 +3975,16 @@
       <c r="G64">
         <f>_xlfn.IFNA(INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0)),"")</f>
         <v/>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>CHE</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>PSG</t>
+        </is>
       </c>
       <c r="J64" s="2" t="n">
         <v>3</v>

</xml_diff>